<commit_message>
added pilot scripts and stimuli
</commit_message>
<xml_diff>
--- a/data/pilot/000/lifetime_run-1.xlsx
+++ b/data/pilot/000/lifetime_run-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haozi\Desktop\PhD\fMRI_PrC-PPC\data\pilot\000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BB66A1-5EBE-42DD-9D87-AFF3A6F2AC2B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419177AE-2140-4B4A-A3BC-E2E97F6E1CF2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="8382" xr2:uid="{4461D55D-71C4-4803-8CB0-F41B756FF41C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="8382" xr2:uid="{253A032A-54A0-4773-9964-F9C633993CD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -540,7 +540,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE252485-14E0-4EB7-AF8E-FA0B242A3750}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB1BB98-8748-4EDD-82C9-4EC225661055}">
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -586,16 +586,19 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2">
-        <v>170298.65658242899</v>
+        <v>32544.446955200001</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>2.5047941708471626</v>
+        <v>0.64923369999814895</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -609,19 +612,16 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3">
-        <v>170307.12703530112</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
+        <v>32552.920392100001</v>
       </c>
       <c r="H3">
-        <v>0.59121054576826282</v>
+        <v>2.5004396999975143</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -635,16 +635,19 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4">
-        <v>170310.4366309772</v>
+        <v>32558.141877099999</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>2.515770057507325</v>
+        <v>0.36716630000228179</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -658,19 +661,19 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
       <c r="F5">
-        <v>170319.04689373274</v>
+        <v>32566.732453100001</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>0.96825007829465903</v>
+        <v>0.88267259999702219</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -684,19 +687,16 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
       </c>
       <c r="F6">
-        <v>170324.01620483337</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
+        <v>32573.247048500001</v>
       </c>
       <c r="H6">
-        <v>0.68634465278591961</v>
+        <v>2.5005311999993864</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -710,7 +710,7 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -727,7 +727,7 @@
         <v>7</v>
       </c>
       <c r="D8">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -744,7 +744,7 @@
         <v>8</v>
       </c>
       <c r="D9">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
@@ -761,7 +761,7 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
@@ -778,7 +778,7 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E11" t="s">
         <v>17</v>
@@ -795,7 +795,7 @@
         <v>11</v>
       </c>
       <c r="D12">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E12" t="s">
         <v>18</v>
@@ -812,7 +812,7 @@
         <v>12</v>
       </c>
       <c r="D13">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E13" t="s">
         <v>19</v>
@@ -829,7 +829,7 @@
         <v>13</v>
       </c>
       <c r="D14">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E14" t="s">
         <v>20</v>
@@ -846,7 +846,7 @@
         <v>14</v>
       </c>
       <c r="D15">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E15" t="s">
         <v>21</v>
@@ -863,7 +863,7 @@
         <v>15</v>
       </c>
       <c r="D16">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E16" t="s">
         <v>22</v>
@@ -880,7 +880,7 @@
         <v>16</v>
       </c>
       <c r="D17">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E17" t="s">
         <v>23</v>
@@ -897,7 +897,7 @@
         <v>17</v>
       </c>
       <c r="D18">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E18" t="s">
         <v>24</v>
@@ -914,7 +914,7 @@
         <v>18</v>
       </c>
       <c r="D19">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E19" t="s">
         <v>25</v>
@@ -931,7 +931,7 @@
         <v>19</v>
       </c>
       <c r="D20">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E20" t="s">
         <v>26</v>
@@ -948,7 +948,7 @@
         <v>20</v>
       </c>
       <c r="D21">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E21" t="s">
         <v>27</v>
@@ -965,7 +965,7 @@
         <v>21</v>
       </c>
       <c r="D22">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E22" t="s">
         <v>28</v>
@@ -982,7 +982,7 @@
         <v>22</v>
       </c>
       <c r="D23">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E23" t="s">
         <v>29</v>
@@ -999,7 +999,7 @@
         <v>23</v>
       </c>
       <c r="D24">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E24" t="s">
         <v>30</v>
@@ -1016,7 +1016,7 @@
         <v>24</v>
       </c>
       <c r="D25">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E25" t="s">
         <v>31</v>
@@ -1033,7 +1033,7 @@
         <v>25</v>
       </c>
       <c r="D26">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E26" t="s">
         <v>32</v>
@@ -1050,7 +1050,7 @@
         <v>26</v>
       </c>
       <c r="D27">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E27" t="s">
         <v>33</v>
@@ -1067,7 +1067,7 @@
         <v>27</v>
       </c>
       <c r="D28">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E28" t="s">
         <v>34</v>
@@ -1084,7 +1084,7 @@
         <v>28</v>
       </c>
       <c r="D29">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E29" t="s">
         <v>35</v>
@@ -1101,7 +1101,7 @@
         <v>29</v>
       </c>
       <c r="D30">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E30" t="s">
         <v>36</v>
@@ -1118,7 +1118,7 @@
         <v>30</v>
       </c>
       <c r="D31">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E31" t="s">
         <v>37</v>
@@ -1135,7 +1135,7 @@
         <v>31</v>
       </c>
       <c r="D32">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E32" t="s">
         <v>38</v>
@@ -1152,7 +1152,7 @@
         <v>32</v>
       </c>
       <c r="D33">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E33" t="s">
         <v>39</v>
@@ -1169,7 +1169,7 @@
         <v>33</v>
       </c>
       <c r="D34">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E34" t="s">
         <v>40</v>
@@ -1186,7 +1186,7 @@
         <v>34</v>
       </c>
       <c r="D35">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E35" t="s">
         <v>41</v>
@@ -1203,7 +1203,7 @@
         <v>35</v>
       </c>
       <c r="D36">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E36" t="s">
         <v>42</v>
@@ -1220,7 +1220,7 @@
         <v>36</v>
       </c>
       <c r="D37">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E37" t="s">
         <v>43</v>
@@ -1237,7 +1237,7 @@
         <v>37</v>
       </c>
       <c r="D38">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E38" t="s">
         <v>44</v>
@@ -1254,7 +1254,7 @@
         <v>38</v>
       </c>
       <c r="D39">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E39" t="s">
         <v>45</v>
@@ -1271,7 +1271,7 @@
         <v>39</v>
       </c>
       <c r="D40">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E40" t="s">
         <v>46</v>
@@ -1288,7 +1288,7 @@
         <v>40</v>
       </c>
       <c r="D41">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E41" t="s">
         <v>47</v>
@@ -1305,7 +1305,7 @@
         <v>41</v>
       </c>
       <c r="D42">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E42" t="s">
         <v>48</v>
@@ -1322,7 +1322,7 @@
         <v>42</v>
       </c>
       <c r="D43">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E43" t="s">
         <v>49</v>
@@ -1339,7 +1339,7 @@
         <v>43</v>
       </c>
       <c r="D44">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E44" t="s">
         <v>50</v>
@@ -1356,7 +1356,7 @@
         <v>44</v>
       </c>
       <c r="D45">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E45" t="s">
         <v>51</v>
@@ -1373,7 +1373,7 @@
         <v>45</v>
       </c>
       <c r="D46">
-        <v>170293.55032292599</v>
+        <v>32539.366537900001</v>
       </c>
       <c r="E46" t="s">
         <v>52</v>

</xml_diff>